<commit_message>
Renamed and optimized code for uniquevalue generation
Signed-off-by: Shivaprasad <cse.shivaprasad@gmail.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/batchconfig/templates/BatchConsumerTransactions.xlsx
+++ b/src/main/resources/batchconfig/templates/BatchConsumerTransactions.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BatchTemplateConfig" sheetId="1" r:id="rId1"/>
-    <sheet name="BatchFieldConfig" sheetId="2" r:id="rId2"/>
+    <sheet name="CustomDataTypes" sheetId="1" r:id="rId1"/>
+    <sheet name="FieldConfig" sheetId="2" r:id="rId2"/>
     <sheet name="StreamTemplateConfig" sheetId="3" r:id="rId3"/>
     <sheet name="StreamFieldConfig" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
   <si>
     <t>jobName</t>
   </si>
@@ -75,9 +75,6 @@
     <t>consumerId</t>
   </si>
   <si>
-    <t>outputConfigPath</t>
-  </si>
-  <si>
     <t>consumerName</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>cardNumber</t>
   </si>
   <si>
-    <t>emailId</t>
-  </si>
-  <si>
     <t>balanceAmt</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>recordCount</t>
-  </si>
-  <si>
     <t>fieldLength</t>
   </si>
   <si>
@@ -150,15 +141,6 @@
     <t>accoutType</t>
   </si>
   <si>
-    <t>PTS Batch File Feed</t>
-  </si>
-  <si>
-    <t>FixedWidth</t>
-  </si>
-  <si>
-    <t>en-US</t>
-  </si>
-  <si>
     <t>RANDOM_LONG</t>
   </si>
   <si>
@@ -211,6 +193,57 @@
   </si>
   <si>
     <t>{POSSIBLE_VALUES:["Saving","HouseLoan","Current"]}</t>
+  </si>
+  <si>
+    <t>VISA_CARD_NUMBER</t>
+  </si>
+  <si>
+    <t>AMEX_CARD_NUMBER</t>
+  </si>
+  <si>
+    <t>FIRST_NAME</t>
+  </si>
+  <si>
+    <t>LAST_NAME</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>{PATTERN:"??????????##@mastercard.com"}</t>
+  </si>
+  <si>
+    <t>en-IND</t>
+  </si>
+  <si>
+    <t>CustomTypes</t>
+  </si>
+  <si>
+    <t>DISCOVER_CARD_NUMBER</t>
+  </si>
+  <si>
+    <t>BANK</t>
+  </si>
+  <si>
+    <t>CURRENCY_CODE</t>
+  </si>
+  <si>
+    <t>currencyCode</t>
+  </si>
+  <si>
+    <t>RANDON_STRING</t>
+  </si>
+  <si>
+    <t>CURRENCY_NAME</t>
+  </si>
+  <si>
+    <t>officeEmailId</t>
+  </si>
+  <si>
+    <t>personalEmail</t>
+  </si>
+  <si>
+    <t>PATTERN_EMAIL</t>
   </si>
 </sst>
 </file>
@@ -242,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +285,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +319,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -300,13 +339,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -316,6 +375,15 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -325,6 +393,15 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -654,59 +731,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -722,10 +879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -733,10 +890,11 @@
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -753,30 +911,33 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2">
@@ -784,43 +945,47 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2">
@@ -828,22 +993,23 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
@@ -852,19 +1018,20 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2">
@@ -872,106 +1039,115 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2">
         <v>30</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
@@ -980,19 +1156,22 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
@@ -1001,63 +1180,66 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
         <v>10</v>
       </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
@@ -1065,14 +1247,71 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="4">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>CustomDataTypes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C7 C9:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>

</xml_diff>

<commit_message>
Optimized HashMap entries code to make use of checkIfAbsent method
Signed-off-by: Shivaprasad <cse.shivaprasad@gmail.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/batchconfig/templates/BatchConsumerTransactions.xlsx
+++ b/src/main/resources/batchconfig/templates/BatchConsumerTransactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CustomDataTypes" sheetId="1" r:id="rId1"/>
@@ -882,7 +882,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">

</xml_diff>